<commit_message>
EPBDS: added the following feature: user can override field mappings for child classes.
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/inheritance/SuperMappingsOrderTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/inheritance/SuperMappingsOrderTest.xlsx
@@ -570,13 +570,13 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="3:6">
@@ -584,13 +584,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>